<commit_message>
TMTT0046984_VerificationOfEngagementCompanyRoundtripFlagFunctionalityOnTheBuysideDeals - Mid - 5th May 2025
</commit_message>
<xml_diff>
--- a/TestData/TMTT0046984_VerificationOfEngagementCompanyRoundtripFlagFunctionalityOnTheBuysideDeals.xlsx
+++ b/TestData/TMTT0046984_VerificationOfEngagementCompanyRoundtripFlagFunctionalityOnTheBuysideDeals.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F7DDA0E-82F0-4AD3-9609-AC61B8B0B8A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F25C9DFF-F41E-47ED-86E6-14FC0DFB4D33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="468" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="468" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="2" r:id="rId1"/>
@@ -254,7 +254,7 @@
     <t>CaoUser</t>
   </si>
   <si>
-    <t>Gemma Hardy</t>
+    <t>Brian Miller</t>
   </si>
 </sst>
 </file>
@@ -587,8 +587,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C8:C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -868,7 +868,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33474F8B-FFCF-4033-9E95-D6C9D3A8099C}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
TMTT0046984_VerificationOfEngagementCompanyRoundtripFlagFunctionalityOnTheBuysideDeals - Final - 5th May 2025
</commit_message>
<xml_diff>
--- a/TestData/TMTT0046984_VerificationOfEngagementCompanyRoundtripFlagFunctionalityOnTheBuysideDeals.xlsx
+++ b/TestData/TMTT0046984_VerificationOfEngagementCompanyRoundtripFlagFunctionalityOnTheBuysideDeals.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F25C9DFF-F41E-47ED-86E6-14FC0DFB4D33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6418223F-99B8-4D57-A8F8-9726F51B2175}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="468" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="468" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="2" r:id="rId1"/>
-    <sheet name="Contact" sheetId="10" r:id="rId2"/>
-    <sheet name="AddOpportunity" sheetId="12" r:id="rId3"/>
-    <sheet name="AddContact" sheetId="13" r:id="rId4"/>
+    <sheet name="PicklistValues" sheetId="14" r:id="rId2"/>
+    <sheet name="Contact" sheetId="10" r:id="rId3"/>
+    <sheet name="AddOpportunity" sheetId="12" r:id="rId4"/>
+    <sheet name="AddContact" sheetId="13" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="76">
   <si>
     <t>Subject</t>
   </si>
@@ -255,6 +256,18 @@
   </si>
   <si>
     <t>Brian Miller</t>
+  </si>
+  <si>
+    <t>EngPotentialRoundTrip PicklistValues</t>
+  </si>
+  <si>
+    <t>Neither subject nor buyer are round trip</t>
+  </si>
+  <si>
+    <t>Subject is a potential round trip</t>
+  </si>
+  <si>
+    <t>Buyer is a potential round trip</t>
   </si>
 </sst>
 </file>
@@ -587,8 +600,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C8:C9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -619,6 +632,44 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB5A9CA0-9D6D-4A18-8830-C9EDB8538004}">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="35.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78F6AD56-19A8-4526-A92B-5BB161C99B6D}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -660,7 +711,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1175537-D85E-4D33-8AD2-B3C163BE409D}">
   <dimension ref="A1:AD2"/>
   <sheetViews>
@@ -864,7 +915,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33474F8B-FFCF-4033-9E95-D6C9D3A8099C}">
   <dimension ref="A1:H2"/>
   <sheetViews>

</xml_diff>

<commit_message>
Final - 5th May 2025
</commit_message>
<xml_diff>
--- a/TestData/TMTT0046984_VerificationOfEngagementCompanyRoundtripFlagFunctionalityOnTheBuysideDeals.xlsx
+++ b/TestData/TMTT0046984_VerificationOfEngagementCompanyRoundtripFlagFunctionalityOnTheBuysideDeals.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6418223F-99B8-4D57-A8F8-9726F51B2175}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B04D3456-BCC7-40C3-9675-5CEA847ED650}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="468" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="468" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="2" r:id="rId1"/>
     <sheet name="PicklistValues" sheetId="14" r:id="rId2"/>
-    <sheet name="Contact" sheetId="10" r:id="rId3"/>
-    <sheet name="AddOpportunity" sheetId="12" r:id="rId4"/>
-    <sheet name="AddContact" sheetId="13" r:id="rId5"/>
+    <sheet name="HoverIcon" sheetId="15" r:id="rId3"/>
+    <sheet name="Contact" sheetId="10" r:id="rId4"/>
+    <sheet name="AddOpportunity" sheetId="12" r:id="rId5"/>
+    <sheet name="AddContact" sheetId="13" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="78">
   <si>
     <t>Subject</t>
   </si>
@@ -268,6 +269,12 @@
   </si>
   <si>
     <t>Buyer is a potential round trip</t>
+  </si>
+  <si>
+    <t>Hover Icon Text</t>
+  </si>
+  <si>
+    <t>An engagement is typically considered a potential round trip if it is acquired by a sponsor (subject is a potential round trip) or by a sponsor-backed operating company (buyer is a potential round trip). Note "sponsor" includes firms tagged as Private Equity Group, Hedge Fund, or Family Office.</t>
   </si>
 </sst>
 </file>
@@ -311,12 +318,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -635,7 +645,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB5A9CA0-9D6D-4A18-8830-C9EDB8538004}">
   <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
@@ -670,6 +680,34 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4729222E-8D4C-4BA0-8280-0499EC9AAD18}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="66" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78F6AD56-19A8-4526-A92B-5BB161C99B6D}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -711,7 +749,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1175537-D85E-4D33-8AD2-B3C163BE409D}">
   <dimension ref="A1:AD2"/>
   <sheetViews>
@@ -915,7 +953,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33474F8B-FFCF-4033-9E95-D6C9D3A8099C}">
   <dimension ref="A1:H2"/>
   <sheetViews>

</xml_diff>

<commit_message>
TMTT0046984_VerificationOfEngagementCompanyRoundtripFlagFunctionalityOnTheBuysideDeals - Mid - 6th May 2025
</commit_message>
<xml_diff>
--- a/TestData/TMTT0046984_VerificationOfEngagementCompanyRoundtripFlagFunctionalityOnTheBuysideDeals.xlsx
+++ b/TestData/TMTT0046984_VerificationOfEngagementCompanyRoundtripFlagFunctionalityOnTheBuysideDeals.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B04D3456-BCC7-40C3-9675-5CEA847ED650}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94D67D56-C171-4924-B282-36433396E0B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="468" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="468" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="2" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="80">
   <si>
     <t>Subject</t>
   </si>
@@ -154,9 +154,6 @@
     <t>WomenLed</t>
   </si>
   <si>
-    <t>Techno Coatings, Inc.</t>
-  </si>
-  <si>
     <t>Buyside</t>
   </si>
   <si>
@@ -178,12 +175,6 @@
     <t>Do Not Disclose</t>
   </si>
   <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>Public Equity</t>
-  </si>
-  <si>
     <t>9999</t>
   </si>
   <si>
@@ -275,6 +266,21 @@
   </si>
   <si>
     <t>An engagement is typically considered a potential round trip if it is acquired by a sponsor (subject is a potential round trip) or by a sponsor-backed operating company (buyer is a potential round trip). Note "sponsor" includes firms tagged as Private Equity Group, Hedge Fund, or Family Office.</t>
+  </si>
+  <si>
+    <t>TPG Global, LLC</t>
+  </si>
+  <si>
+    <t>Poundworld Retail Ltd.</t>
+  </si>
+  <si>
+    <t>Private Equity Group</t>
+  </si>
+  <si>
+    <t>Family Office</t>
+  </si>
+  <si>
+    <t>1000</t>
   </si>
 </sst>
 </file>
@@ -621,18 +627,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -656,22 +662,22 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -683,7 +689,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4729222E-8D4C-4BA0-8280-0499EC9AAD18}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -694,12 +700,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -753,12 +759,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1175537-D85E-4D33-8AD2-B3C163BE409D}">
   <dimension ref="A1:AD2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="Z10" sqref="Z10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="18" customWidth="1"/>
+    <col min="2" max="2" width="21.77734375" customWidth="1"/>
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.88671875" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="23.6640625" customWidth="1"/>
@@ -858,94 +866,94 @@
     </row>
     <row r="2" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C2" t="s">
         <v>37</v>
-      </c>
-      <c r="B2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C2" t="s">
-        <v>38</v>
       </c>
       <c r="D2" t="s">
         <v>1</v>
       </c>
       <c r="E2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F2" t="s">
         <v>39</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H2" t="s">
         <v>40</v>
       </c>
-      <c r="G2" t="s">
-        <v>40</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
+        <v>39</v>
+      </c>
+      <c r="J2" t="s">
+        <v>39</v>
+      </c>
+      <c r="K2" t="s">
         <v>41</v>
       </c>
-      <c r="I2" t="s">
-        <v>40</v>
-      </c>
-      <c r="J2" t="s">
-        <v>40</v>
-      </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>42</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>43</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
+        <v>66</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="R2" t="s">
+        <v>77</v>
+      </c>
+      <c r="S2" t="s">
+        <v>78</v>
+      </c>
+      <c r="T2" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="N2" t="s">
-        <v>69</v>
-      </c>
-      <c r="O2" s="3" t="s">
+      <c r="U2" t="s">
         <v>45</v>
       </c>
-      <c r="P2" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q2" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="R2" t="s">
+      <c r="V2" t="s">
         <v>46</v>
       </c>
-      <c r="S2" t="s">
-        <v>46</v>
-      </c>
-      <c r="T2" s="3" t="s">
+      <c r="W2" t="s">
         <v>47</v>
       </c>
-      <c r="U2" t="s">
+      <c r="X2" t="s">
         <v>48</v>
       </c>
-      <c r="V2" t="s">
+      <c r="Y2" t="s">
         <v>49</v>
       </c>
-      <c r="W2" t="s">
+      <c r="Z2" t="s">
         <v>50</v>
       </c>
-      <c r="X2" t="s">
+      <c r="AA2" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB2" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>66</v>
+      </c>
+      <c r="AD2" t="s">
         <v>51</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>52</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>53</v>
-      </c>
-      <c r="AA2" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="AB2" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>69</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -965,54 +973,54 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E2" t="s">
         <v>8</v>
       </c>
       <c r="F2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="G2" t="s">
         <v>8</v>
       </c>
       <c r="H2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
TMTT0046984_VerificationOfEngagementCompanyRoundtripFlagFunctionalityOnTheBuysideDeals - Mid - 7th May 2025
</commit_message>
<xml_diff>
--- a/TestData/TMTT0046984_VerificationOfEngagementCompanyRoundtripFlagFunctionalityOnTheBuysideDeals.xlsx
+++ b/TestData/TMTT0046984_VerificationOfEngagementCompanyRoundtripFlagFunctionalityOnTheBuysideDeals.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94D67D56-C171-4924-B282-36433396E0B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BBCEE14-0CB9-4DE2-BD76-562E209A25AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="468" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="568" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="2" r:id="rId1"/>
@@ -18,7 +18,8 @@
     <sheet name="HoverIcon" sheetId="15" r:id="rId3"/>
     <sheet name="Contact" sheetId="10" r:id="rId4"/>
     <sheet name="AddOpportunity" sheetId="12" r:id="rId5"/>
-    <sheet name="AddContact" sheetId="13" r:id="rId6"/>
+    <sheet name="CompanyUpdates" sheetId="16" r:id="rId6"/>
+    <sheet name="AddContact" sheetId="13" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="84">
   <si>
     <t>Subject</t>
   </si>
@@ -281,6 +282,18 @@
   </si>
   <si>
     <t>1000</t>
+  </si>
+  <si>
+    <t>Round Trip Comment</t>
+  </si>
+  <si>
+    <t>Source - Engagement</t>
+  </si>
+  <si>
+    <t>Subject Potential Round Trip</t>
+  </si>
+  <si>
+    <t>Client Potential Round Trip</t>
   </si>
 </sst>
 </file>
@@ -324,7 +337,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -333,6 +346,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -759,7 +775,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1175537-D85E-4D33-8AD2-B3C163BE409D}">
   <dimension ref="A1:AD2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+    <sheetView topLeftCell="N1" workbookViewId="0">
       <selection activeCell="Z10" sqref="Z10"/>
     </sheetView>
   </sheetViews>
@@ -962,6 +978,48 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C30D5517-1C18-480A-9228-B12CD8B6EC9B}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="25.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.21875" customWidth="1"/>
+    <col min="3" max="3" width="23.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33474F8B-FFCF-4033-9E95-D6C9D3A8099C}">
   <dimension ref="A1:H2"/>
   <sheetViews>

</xml_diff>

<commit_message>
TMTT0046984_VerificationOfEngagementCompanyRoundtripFlagFunctionalityOnTheBuysideDeals - Mid - 7th May
</commit_message>
<xml_diff>
--- a/TestData/TMTT0046984_VerificationOfEngagementCompanyRoundtripFlagFunctionalityOnTheBuysideDeals.xlsx
+++ b/TestData/TMTT0046984_VerificationOfEngagementCompanyRoundtripFlagFunctionalityOnTheBuysideDeals.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BBCEE14-0CB9-4DE2-BD76-562E209A25AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EAF6577-F372-41AA-ABA9-5985BFCEC487}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="568" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="568" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="2" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="87">
   <si>
     <t>Subject</t>
   </si>
@@ -294,6 +294,15 @@
   </si>
   <si>
     <t>Client Potential Round Trip</t>
+  </si>
+  <si>
+    <t>Pharmavite, LLC</t>
+  </si>
+  <si>
+    <t>Food State, Inc.</t>
+  </si>
+  <si>
+    <t>Hedge Fund</t>
   </si>
 </sst>
 </file>
@@ -773,10 +782,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1175537-D85E-4D33-8AD2-B3C163BE409D}">
-  <dimension ref="A1:AD2"/>
+  <dimension ref="A1:AD3"/>
   <sheetViews>
-    <sheetView topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="Z10" sqref="Z10"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="R9" sqref="R9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -785,6 +794,7 @@
     <col min="2" max="2" width="21.77734375" customWidth="1"/>
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.88671875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.77734375" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="23.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -969,6 +979,98 @@
         <v>66</v>
       </c>
       <c r="AD2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G3" t="s">
+        <v>39</v>
+      </c>
+      <c r="H3" t="s">
+        <v>40</v>
+      </c>
+      <c r="I3" t="s">
+        <v>39</v>
+      </c>
+      <c r="J3" t="s">
+        <v>39</v>
+      </c>
+      <c r="K3" t="s">
+        <v>41</v>
+      </c>
+      <c r="L3" t="s">
+        <v>42</v>
+      </c>
+      <c r="M3" t="s">
+        <v>43</v>
+      </c>
+      <c r="N3" t="s">
+        <v>66</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="R3" t="s">
+        <v>86</v>
+      </c>
+      <c r="S3" t="s">
+        <v>78</v>
+      </c>
+      <c r="T3" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="U3" t="s">
+        <v>45</v>
+      </c>
+      <c r="V3" t="s">
+        <v>46</v>
+      </c>
+      <c r="W3" t="s">
+        <v>47</v>
+      </c>
+      <c r="X3" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>50</v>
+      </c>
+      <c r="AA3" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB3" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>66</v>
+      </c>
+      <c r="AD3" t="s">
         <v>51</v>
       </c>
     </row>
@@ -981,7 +1083,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C30D5517-1C18-480A-9228-B12CD8B6EC9B}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
TMTT0046984_VerificationOfEngagementCompanyRoundtripFlagFunctionalityOnTheBuysideDeals - Initial - 12 May 2025
</commit_message>
<xml_diff>
--- a/TestData/TMTT0046984_VerificationOfEngagementCompanyRoundtripFlagFunctionalityOnTheBuysideDeals.xlsx
+++ b/TestData/TMTT0046984_VerificationOfEngagementCompanyRoundtripFlagFunctionalityOnTheBuysideDeals.xlsx
@@ -8,18 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EAF6577-F372-41AA-ABA9-5985BFCEC487}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF68B41A-F353-4248-B390-64F99047C254}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="568" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="568" firstSheet="3" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="2" r:id="rId1"/>
     <sheet name="PicklistValues" sheetId="14" r:id="rId2"/>
     <sheet name="HoverIcon" sheetId="15" r:id="rId3"/>
     <sheet name="Contact" sheetId="10" r:id="rId4"/>
-    <sheet name="AddOpportunity" sheetId="12" r:id="rId5"/>
-    <sheet name="CompanyUpdates" sheetId="16" r:id="rId6"/>
-    <sheet name="AddContact" sheetId="13" r:id="rId7"/>
+    <sheet name="Warning" sheetId="17" r:id="rId5"/>
+    <sheet name="AddOpportunity" sheetId="12" r:id="rId6"/>
+    <sheet name="CompanyUpdates" sheetId="16" r:id="rId7"/>
+    <sheet name="AddContact" sheetId="13" r:id="rId8"/>
+    <sheet name="FlagReason" sheetId="18" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -42,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="93">
   <si>
     <t>Subject</t>
   </si>
@@ -303,6 +305,24 @@
   </si>
   <si>
     <t>Hedge Fund</t>
+  </si>
+  <si>
+    <t>Warning Msg</t>
+  </si>
+  <si>
+    <t>A Subject is typically considered a potential round trip if it is an operating company acquired either by a Private Equity firm or by a PE-owned operating company. The Subject is not listed as an Operating Company. If you still want to consider them a round trip candidate no change is needed; otherwise, please change the selection.</t>
+  </si>
+  <si>
+    <t>Reason</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>Requesting to change Company Type to Operating Company because it is being considered to be a potential round trip</t>
+  </si>
+  <si>
+    <t>Change Company Type</t>
   </si>
 </sst>
 </file>
@@ -346,7 +366,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -358,6 +378,18 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -781,10 +813,38 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{428EFC0A-BA50-4449-A054-B06ABB328678}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="67.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="72" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1175537-D85E-4D33-8AD2-B3C163BE409D}">
   <dimension ref="A1:AD3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="R9" sqref="R9"/>
     </sheetView>
   </sheetViews>
@@ -1079,7 +1139,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C30D5517-1C18-480A-9228-B12CD8B6EC9B}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -1121,7 +1181,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33474F8B-FFCF-4033-9E95-D6C9D3A8099C}">
   <dimension ref="A1:H2"/>
   <sheetViews>
@@ -1186,4 +1246,39 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92EA0090-8A70-4EE9-9BBD-D73C51089E4F}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="32.44140625" customWidth="1"/>
+    <col min="2" max="2" width="56" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>91</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
TMTT0046984_VerificationOfEngagementCompanyRoundtripFlagFunctionalityOnTheBuysideDeals - Mid - 13 May 2025
</commit_message>
<xml_diff>
--- a/TestData/TMTT0046984_VerificationOfEngagementCompanyRoundtripFlagFunctionalityOnTheBuysideDeals.xlsx
+++ b/TestData/TMTT0046984_VerificationOfEngagementCompanyRoundtripFlagFunctionalityOnTheBuysideDeals.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF68B41A-F353-4248-B390-64F99047C254}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C386CF55-159C-45F5-925C-538D8E80FB03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="568" firstSheet="3" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="568" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="2" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="93">
   <si>
     <t>Subject</t>
   </si>
@@ -1141,10 +1141,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C30D5517-1C18-480A-9228-B12CD8B6EC9B}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1173,6 +1173,17 @@
         <v>81</v>
       </c>
       <c r="C2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C3" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1252,7 +1263,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92EA0090-8A70-4EE9-9BBD-D73C51089E4F}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
TMTT0046984_VerificationOfEngagementCompanyRoundtripFlagFunctionalityOnTheBuysideDeals - Final - 13 May 2025
</commit_message>
<xml_diff>
--- a/TestData/TMTT0046984_VerificationOfEngagementCompanyRoundtripFlagFunctionalityOnTheBuysideDeals.xlsx
+++ b/TestData/TMTT0046984_VerificationOfEngagementCompanyRoundtripFlagFunctionalityOnTheBuysideDeals.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C386CF55-159C-45F5-925C-538D8E80FB03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C1660A7-D546-45BD-9F0E-E08379BE38B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="568" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="568" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="2" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="96">
   <si>
     <t>Subject</t>
   </si>
@@ -323,6 +323,15 @@
   </si>
   <si>
     <t>Change Company Type</t>
+  </si>
+  <si>
+    <t>Team, Inc</t>
+  </si>
+  <si>
+    <t>QualSpec Group</t>
+  </si>
+  <si>
+    <t>Private Equity</t>
   </si>
 </sst>
 </file>
@@ -842,10 +851,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1175537-D85E-4D33-8AD2-B3C163BE409D}">
-  <dimension ref="A1:AD3"/>
+  <dimension ref="A1:AD4"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="R9" sqref="R9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="V12" sqref="V12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -855,6 +864,7 @@
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.88671875" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.44140625" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="23.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1131,6 +1141,98 @@
         <v>66</v>
       </c>
       <c r="AD3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G4" t="s">
+        <v>39</v>
+      </c>
+      <c r="H4" t="s">
+        <v>40</v>
+      </c>
+      <c r="I4" t="s">
+        <v>39</v>
+      </c>
+      <c r="J4" t="s">
+        <v>39</v>
+      </c>
+      <c r="K4" t="s">
+        <v>41</v>
+      </c>
+      <c r="L4" t="s">
+        <v>42</v>
+      </c>
+      <c r="M4" t="s">
+        <v>43</v>
+      </c>
+      <c r="N4" t="s">
+        <v>66</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q4" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="R4" t="s">
+        <v>95</v>
+      </c>
+      <c r="S4" t="s">
+        <v>78</v>
+      </c>
+      <c r="T4" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="U4" t="s">
+        <v>45</v>
+      </c>
+      <c r="V4" t="s">
+        <v>46</v>
+      </c>
+      <c r="W4" t="s">
+        <v>47</v>
+      </c>
+      <c r="X4" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>50</v>
+      </c>
+      <c r="AA4" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB4" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>66</v>
+      </c>
+      <c r="AD4" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1141,10 +1243,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C30D5517-1C18-480A-9228-B12CD8B6EC9B}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1184,6 +1286,17 @@
         <v>81</v>
       </c>
       <c r="C3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C4" t="s">
         <v>39</v>
       </c>
     </row>

</xml_diff>